<commit_message>
Fix dropdown button AddAPITest
</commit_message>
<xml_diff>
--- a/automation-testing/src/test/resources/data_source.xlsx
+++ b/automation-testing/src/test/resources/data_source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CSC13003-Software-Testing\automation-testing\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47467C32-A57E-4CB3-ADA0-9BFA5F9FECC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A86D15-C4EE-4E9A-A7A4-A44D15A82738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="26">
   <si>
     <t>No</t>
   </si>
@@ -66,6 +66,46 @@
   <si>
     <t>Successfully Saved
 Navigate to "searchKPI" page</t>
+  </si>
+  <si>
+    <t>Tracker Name</t>
+  </si>
+  <si>
+    <t>Employee Name</t>
+  </si>
+  <si>
+    <t>First Quarter 2022</t>
+  </si>
+  <si>
+    <t>Hà My Nguyễn</t>
+  </si>
+  <si>
+    <t>Minh Châu Nguyễn</t>
+  </si>
+  <si>
+    <t>http://localhost/orangehrm-5.1/web/index.php/performance/viewPerformanceTracker</t>
+  </si>
+  <si>
+    <t>1 error field</t>
+  </si>
+  <si>
+    <t>Minh Anh Nguyễn</t>
+  </si>
+  <si>
+    <t>2 error field</t>
+  </si>
+  <si>
+    <t>Hà My Nguyễn, Linh Trang Phạm</t>
+  </si>
+  <si>
+    <t>Minh Châu Nguyễn
+Linh Trang Phạm</t>
+  </si>
+  <si>
+    <t>Reviewers Name</t>
+  </si>
+  <si>
+    <t>Marketing</t>
   </si>
 </sst>
 </file>
@@ -108,10 +148,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -397,14 +440,14 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="89.625" style="1" bestFit="1" customWidth="1"/>
@@ -570,7 +613,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
@@ -701,12 +744,195 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5202BB-CAED-4C18-BF61-942CC1D604C0}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="5.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="31.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="89.5" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Create test case Add Performance Tracker Page
</commit_message>
<xml_diff>
--- a/automation-testing/src/test/resources/data_source.xlsx
+++ b/automation-testing/src/test/resources/data_source.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CSC13003-Software-Testing\automation-testing\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A86D15-C4EE-4E9A-A7A4-A44D15A82738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED6F435-F3AB-4655-ACEB-A48C624C32C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5925" yWindow="2460" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" r:id="rId1"/>
@@ -95,17 +95,16 @@
     <t>2 error field</t>
   </si>
   <si>
-    <t>Hà My Nguyễn, Linh Trang Phạm</t>
-  </si>
-  <si>
-    <t>Minh Châu Nguyễn
-Linh Trang Phạm</t>
-  </si>
-  <si>
     <t>Reviewers Name</t>
   </si>
   <si>
     <t>Marketing</t>
+  </si>
+  <si>
+    <t>Minh Châu @ Nguyễn</t>
+  </si>
+  <si>
+    <t>Hà My # Nguyễn</t>
   </si>
 </sst>
 </file>
@@ -148,13 +147,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -439,7 +435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -613,7 +609,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
@@ -746,15 +742,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5202BB-CAED-4C18-BF61-942CC1D604C0}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="31.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="89.5" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
@@ -770,7 +767,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
@@ -789,7 +786,7 @@
       <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -897,7 +894,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -905,7 +902,7 @@
         <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>17</v>
@@ -914,7 +911,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -924,11 +921,11 @@
       <c r="C11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>18</v>
+      <c r="D11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>